<commit_message>
SI4463 + I2C kod
Lade till massa filer från Hans Erik som handlade om radion. Har även skrivit massa kod till att prata I2C. Kommunikation fungerar nu med både radion och Acc med SPI.
</commit_message>
<xml_diff>
--- a/Övrigt/Nätlista min version.xlsx
+++ b/Övrigt/Nätlista min version.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="147">
   <si>
     <t>RA0/C12IN0-/AN0</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Radion:</t>
   </si>
   <si>
-    <t>RE3/MCLR/VPP</t>
-  </si>
-  <si>
     <t>GPIO0</t>
   </si>
   <si>
@@ -213,7 +210,253 @@
     <t>SDN</t>
   </si>
   <si>
-    <t>Kopplingar på MCU'n (28 pinnars)</t>
+    <t>RD0/SCK2/SCL2/AN20</t>
+  </si>
+  <si>
+    <t>RD2/P2B/AN22</t>
+  </si>
+  <si>
+    <t>RD1/CCP4/SDI2/SDA2/AN21</t>
+  </si>
+  <si>
+    <t>RD3/P2C/SS2/AN23</t>
+  </si>
+  <si>
+    <t>RD4/P2D/SDO2/AN24</t>
+  </si>
+  <si>
+    <t>RD5/P1B/AN25</t>
+  </si>
+  <si>
+    <t>RD6/P1C/TX2/CK2/AN26</t>
+  </si>
+  <si>
+    <t>RD7/P1D/RX2/DT2/AN27</t>
+  </si>
+  <si>
+    <t>RE0/P3A/CCP3/AN5</t>
+  </si>
+  <si>
+    <t>RE1/P3B/AN6</t>
+  </si>
+  <si>
+    <t>RE2/CCP5/AN7</t>
+  </si>
+  <si>
+    <t>RE3/VPP/MCLR</t>
+  </si>
+  <si>
+    <t>I/O port</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Chip Select</t>
+  </si>
+  <si>
+    <t>En ledig pinne på processorn</t>
+  </si>
+  <si>
+    <t>Kopplas till matningsspänning</t>
+  </si>
+  <si>
+    <t>GPIO2</t>
+  </si>
+  <si>
+    <t>GPIO3</t>
+  </si>
+  <si>
+    <t>Shut down</t>
+  </si>
+  <si>
+    <t>Går nog inte att använda, används för att programmera kortet.</t>
+  </si>
+  <si>
+    <t>Microkontroller</t>
+  </si>
+  <si>
+    <t>RA1</t>
+  </si>
+  <si>
+    <t>RA2</t>
+  </si>
+  <si>
+    <t>RA3</t>
+  </si>
+  <si>
+    <t>RA4</t>
+  </si>
+  <si>
+    <t>RA5</t>
+  </si>
+  <si>
+    <t>RA6</t>
+  </si>
+  <si>
+    <t>RA7</t>
+  </si>
+  <si>
+    <t>RB0</t>
+  </si>
+  <si>
+    <t>RB1</t>
+  </si>
+  <si>
+    <t>RB2</t>
+  </si>
+  <si>
+    <t>RB3</t>
+  </si>
+  <si>
+    <t>RB4</t>
+  </si>
+  <si>
+    <t>RB5</t>
+  </si>
+  <si>
+    <t>RB6</t>
+  </si>
+  <si>
+    <t>RB7</t>
+  </si>
+  <si>
+    <t>RA0</t>
+  </si>
+  <si>
+    <t>RC0</t>
+  </si>
+  <si>
+    <t>RC1</t>
+  </si>
+  <si>
+    <t>RC2</t>
+  </si>
+  <si>
+    <t>RC3</t>
+  </si>
+  <si>
+    <t>RC4</t>
+  </si>
+  <si>
+    <t>RC5</t>
+  </si>
+  <si>
+    <t>RC6</t>
+  </si>
+  <si>
+    <t>RC7</t>
+  </si>
+  <si>
+    <t>RD0</t>
+  </si>
+  <si>
+    <t>RD1</t>
+  </si>
+  <si>
+    <t>RD2</t>
+  </si>
+  <si>
+    <t>RD3</t>
+  </si>
+  <si>
+    <t>RD4</t>
+  </si>
+  <si>
+    <t>RD5</t>
+  </si>
+  <si>
+    <t>RD6</t>
+  </si>
+  <si>
+    <t>RD7</t>
+  </si>
+  <si>
+    <t>RE0</t>
+  </si>
+  <si>
+    <t>RE1</t>
+  </si>
+  <si>
+    <t>RE2</t>
+  </si>
+  <si>
+    <t>RE3</t>
+  </si>
+  <si>
+    <t>Hall sensorn:</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>OUTPUT</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Kopplas till ledig pinne på MCU</t>
+  </si>
+  <si>
+    <t>Matnings LDO:</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>VSEL1</t>
+  </si>
+  <si>
+    <t>VSEL2</t>
+  </si>
+  <si>
+    <t>VSEL3</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>VOS</t>
+  </si>
+  <si>
+    <t>Voltage select 1</t>
+  </si>
+  <si>
+    <t>Power supply</t>
+  </si>
+  <si>
+    <t>Batteriet</t>
+  </si>
+  <si>
+    <t>Kopplas till Vss</t>
+  </si>
+  <si>
+    <t>Switching output</t>
+  </si>
+  <si>
+    <t>Kopplas också till output</t>
+  </si>
+  <si>
+    <t>Feedback voltage</t>
+  </si>
+  <si>
+    <t>Voltage select 3</t>
+  </si>
+  <si>
+    <t>Voltage select 2</t>
+  </si>
+  <si>
+    <t>Master clear</t>
+  </si>
+  <si>
+    <t>Kopplas till en av programmerinspinnarna</t>
+  </si>
+  <si>
+    <t>Kopplingar på MCU'n (40 pinnars)</t>
   </si>
 </sst>
 </file>
@@ -250,7 +493,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -322,12 +565,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -340,6 +664,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Kontrollcell" xfId="1" builtinId="23"/>
@@ -635,16 +973,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:T52"/>
+  <dimension ref="B1:T86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="44.7109375" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -652,31 +990,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:9" ht="16.5" thickTop="1" thickBot="1">
+    <row r="2" spans="2:9" ht="15.75" thickTop="1">
       <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickTop="1">
+    <row r="3" spans="2:9">
       <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -754,20 +1092,29 @@
       <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>24</v>
+      <c r="G9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="2:9">
       <c r="B10" t="s">
         <v>2</v>
       </c>
+      <c r="G10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1">
       <c r="B11" t="s">
@@ -809,8 +1156,8 @@
       <c r="H14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>53</v>
+      <c r="I14" s="14" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="2:9">
@@ -860,104 +1207,641 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="16.5" thickTop="1" thickBot="1">
+    <row r="19" spans="2:9" ht="15.75" thickTop="1">
       <c r="B19" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15.75" thickTop="1">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="H20" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="21" spans="2:9">
-      <c r="G21" t="s">
+      <c r="G21" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="G22" t="s">
-        <v>57</v>
+      <c r="G22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:9">
       <c r="B23" t="s">
         <v>39</v>
       </c>
-      <c r="G23" t="s">
-        <v>58</v>
+      <c r="G23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="2:9">
       <c r="B24" t="s">
         <v>40</v>
       </c>
-      <c r="G24" t="s">
-        <v>59</v>
+      <c r="G24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="2:9">
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="G25" t="s">
-        <v>60</v>
+      <c r="G25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="2:9">
       <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="G26" t="s">
-        <v>61</v>
+      <c r="G26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>43</v>
       </c>
-      <c r="G27" t="s">
-        <v>62</v>
+      <c r="G27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>44</v>
       </c>
-      <c r="G28" t="s">
-        <v>63</v>
+      <c r="G28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="2:9">
       <c r="B29" t="s">
         <v>45</v>
       </c>
-      <c r="G29" t="s">
-        <v>64</v>
+      <c r="G29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="G30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="2:9">
       <c r="B31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="20:20">
+        <v>64</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" thickTop="1">
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H36" s="3"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" s="3"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="G39" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H39" s="3"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H40" s="3"/>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" t="s">
+        <v>73</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H41" s="3"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" t="s">
+        <v>74</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H42" s="3"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H43" s="3"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="G44" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H44" s="3"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="G45" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45" s="3"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="G46" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" s="3"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="2:9">
+      <c r="G47" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H47" s="3"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="2:9">
+      <c r="G48" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H48" s="3"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="7:20">
+      <c r="G49" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H49" s="3"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="7:20">
+      <c r="G50" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H50" s="3"/>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="7:20">
+      <c r="G51" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H51" s="3"/>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="7:20">
+      <c r="G52" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H52" s="3"/>
+      <c r="I52" s="4"/>
       <c r="T52" s="1"/>
+    </row>
+    <row r="53" spans="7:20">
+      <c r="G53" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="7:20">
+      <c r="G54" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H54" s="3"/>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="7:20">
+      <c r="G55" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="H55" s="3"/>
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="7:20">
+      <c r="G56" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H56" s="3"/>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="7:20">
+      <c r="G57" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H57" s="3"/>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="7:20">
+      <c r="G58" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="H58" s="3"/>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="7:20">
+      <c r="G59" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H59" s="3"/>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="7:20">
+      <c r="G60" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H60" s="3"/>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="7:20">
+      <c r="G61" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H61" s="3"/>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="7:20">
+      <c r="G62" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H62" s="3"/>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="7:20">
+      <c r="G63" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H63" s="3"/>
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="7:20">
+      <c r="G64" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H64" s="3"/>
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="7:9">
+      <c r="G65" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H65" s="3"/>
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="7:9">
+      <c r="G66" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="H66" s="3"/>
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="7:9">
+      <c r="G67" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H67" s="3"/>
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="7:9">
+      <c r="G68" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H68" s="3"/>
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="7:9">
+      <c r="G69" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="7:9" ht="15.75" thickBot="1"/>
+    <row r="72" spans="7:9" ht="15.75" thickTop="1">
+      <c r="G72" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="7:9">
+      <c r="G73" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H73" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I73" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="7:9">
+      <c r="G74" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="7:9">
+      <c r="G75" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="7:9">
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="7:9" ht="15.75" thickBot="1">
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+    </row>
+    <row r="78" spans="7:9" ht="15.75" thickTop="1">
+      <c r="G78" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I78" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="7:9">
+      <c r="G79" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H79" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I79" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="7:9">
+      <c r="G80" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="7:9">
+      <c r="G81" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="82" spans="7:9">
+      <c r="G82" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="H82" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" spans="7:9">
+      <c r="G83" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="I83" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="84" spans="7:9">
+      <c r="G84" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="85" spans="7:9">
+      <c r="G85" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="H85" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="86" spans="7:9">
+      <c r="G86" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I86" s="7" t="s">
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>